<commit_message>
Added all of the funcinality of creating worksheets
</commit_message>
<xml_diff>
--- a/PythonApplication1/2022_Wholesale_Delivered_Prices.xlsx
+++ b/PythonApplication1/2022_Wholesale_Delivered_Prices.xlsx
@@ -679,8 +679,8 @@
   </sheetPr>
   <dimension ref="A1:AC241"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.42578125" defaultRowHeight="15"/>

</xml_diff>